<commit_message>
Final sürüm: Tam QoS destegi
</commit_message>
<xml_diff>
--- a/Proje_Sonuclari.xlsx
+++ b/Proje_Sonuclari.xlsx
@@ -519,31 +519,31 @@
         <v>5.4686</v>
       </c>
       <c r="E2" t="n">
-        <v>7.46008</v>
+        <v>8.624680000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>17.874</v>
+        <v>21.554</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9050860000000001</v>
+        <v>0.8807539999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>89.32299613952637</v>
+        <v>669.5258617401123</v>
       </c>
       <c r="I2" t="n">
-        <v>5.9223</v>
+        <v>10.1768</v>
       </c>
       <c r="J2" t="n">
-        <v>10.91116</v>
+        <v>14.612</v>
       </c>
       <c r="K2" t="n">
-        <v>26.886</v>
+        <v>36.076</v>
       </c>
       <c r="L2" t="n">
-        <v>0.894904</v>
+        <v>0.8619600000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>630.0671100616455</v>
+        <v>2843.272876739502</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -562,38 +562,38 @@
         <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>5.429</v>
+        <v>3.386</v>
       </c>
       <c r="E3" t="n">
-        <v>6.691340000000001</v>
+        <v>5.3949</v>
       </c>
       <c r="F3" t="n">
-        <v>17.624</v>
+        <v>14.306</v>
       </c>
       <c r="G3" t="n">
-        <v>0.94086</v>
+        <v>0.940072</v>
       </c>
       <c r="H3" t="n">
-        <v>72.85842895507812</v>
+        <v>608.8993549346924</v>
       </c>
       <c r="I3" t="n">
-        <v>5.429</v>
+        <v>3.8481</v>
       </c>
       <c r="J3" t="n">
-        <v>8.786559999999998</v>
+        <v>5.112819999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>21.306</v>
+        <v>13.652</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9198999999999999</v>
+        <v>0.9484000000000001</v>
       </c>
       <c r="M3" t="n">
-        <v>508.1907272338867</v>
+        <v>1628.496551513672</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>RL</t>
         </is>
       </c>
     </row>
@@ -611,31 +611,31 @@
         <v>4.4996</v>
       </c>
       <c r="E4" t="n">
-        <v>8.09768</v>
+        <v>6.3658</v>
       </c>
       <c r="F4" t="n">
-        <v>19.644</v>
+        <v>15.504</v>
       </c>
       <c r="G4" t="n">
-        <v>0.931466</v>
+        <v>0.909648</v>
       </c>
       <c r="H4" t="n">
-        <v>91.96963310241699</v>
+        <v>715.1021480560303</v>
       </c>
       <c r="I4" t="n">
-        <v>9.6911</v>
+        <v>7.1804</v>
       </c>
       <c r="J4" t="n">
-        <v>13.3952</v>
+        <v>10.75832</v>
       </c>
       <c r="K4" t="n">
-        <v>31.46</v>
+        <v>28.796</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8694900000000001</v>
+        <v>0.902042</v>
       </c>
       <c r="M4" t="n">
-        <v>602.5558471679688</v>
+        <v>2031.07533454895</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -654,34 +654,34 @@
         <v>145</v>
       </c>
       <c r="D5" t="n">
-        <v>5.4766</v>
+        <v>5.6</v>
       </c>
       <c r="E5" t="n">
-        <v>7.002220000000001</v>
+        <v>7.8349</v>
       </c>
       <c r="F5" t="n">
-        <v>17.54</v>
+        <v>18.148</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9547779999999999</v>
+        <v>0.9060159999999999</v>
       </c>
       <c r="H5" t="n">
-        <v>90.79055786132812</v>
+        <v>655.912446975708</v>
       </c>
       <c r="I5" t="n">
-        <v>12.6121</v>
+        <v>7.1637</v>
       </c>
       <c r="J5" t="n">
-        <v>14.3911</v>
+        <v>14.6181</v>
       </c>
       <c r="K5" t="n">
-        <v>33.948</v>
+        <v>34.204</v>
       </c>
       <c r="L5" t="n">
-        <v>0.850516</v>
+        <v>0.8840440000000001</v>
       </c>
       <c r="M5" t="n">
-        <v>688.5376453399658</v>
+        <v>6420.91588973999</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -700,38 +700,38 @@
         <v>10</v>
       </c>
       <c r="D6" t="n">
-        <v>4.2564</v>
+        <v>6.7289</v>
       </c>
       <c r="E6" t="n">
-        <v>5.68336</v>
+        <v>9.96134</v>
       </c>
       <c r="F6" t="n">
-        <v>13.74</v>
+        <v>26.194</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9474879999999999</v>
+        <v>0.900732</v>
       </c>
       <c r="H6" t="n">
-        <v>75.55890083312988</v>
+        <v>662.5673294067383</v>
       </c>
       <c r="I6" t="n">
-        <v>4.2564</v>
+        <v>8.0794</v>
       </c>
       <c r="J6" t="n">
-        <v>4.2564</v>
+        <v>11.11402</v>
       </c>
       <c r="K6" t="n">
-        <v>10</v>
+        <v>28.84</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9719999999999999</v>
+        <v>0.855166</v>
       </c>
       <c r="M6" t="n">
-        <v>324.5217323303223</v>
+        <v>4188.806533813477</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>RL</t>
+          <t>GA</t>
         </is>
       </c>
     </row>
@@ -749,35 +749,35 @@
         <v>2.4773</v>
       </c>
       <c r="E7" t="n">
-        <v>4.166700000000001</v>
+        <v>3.07964</v>
       </c>
       <c r="F7" t="n">
-        <v>9.972</v>
+        <v>7.612</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9680899999999999</v>
+        <v>0.9681899999999999</v>
       </c>
       <c r="H7" t="n">
-        <v>78.52640151977539</v>
+        <v>471.0758686065674</v>
       </c>
       <c r="I7" t="n">
         <v>2.4773</v>
       </c>
       <c r="J7" t="n">
-        <v>3.89948</v>
+        <v>6.42204</v>
       </c>
       <c r="K7" t="n">
-        <v>8.559999999999999</v>
+        <v>16.044</v>
       </c>
       <c r="L7" t="n">
-        <v>0.9648559999999999</v>
+        <v>0.945492</v>
       </c>
       <c r="M7" t="n">
-        <v>433.8950157165527</v>
+        <v>1787.259960174561</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>RL</t>
+          <t>GA</t>
         </is>
       </c>
     </row>
@@ -792,38 +792,38 @@
         <v>232</v>
       </c>
       <c r="D8" t="n">
-        <v>3.0447</v>
+        <v>6.181</v>
       </c>
       <c r="E8" t="n">
-        <v>4.929460000000001</v>
+        <v>9.598560000000001</v>
       </c>
       <c r="F8" t="n">
-        <v>10.24</v>
+        <v>25.056</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9206420000000002</v>
+        <v>0.9224200000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>70.99032402038574</v>
+        <v>481.5999031066895</v>
       </c>
       <c r="I8" t="n">
-        <v>3.0447</v>
+        <v>3.903</v>
       </c>
       <c r="J8" t="n">
-        <v>7.157680000000001</v>
+        <v>8.88748</v>
       </c>
       <c r="K8" t="n">
-        <v>15.78</v>
+        <v>22.366</v>
       </c>
       <c r="L8" t="n">
-        <v>0.930744</v>
+        <v>0.8621800000000001</v>
       </c>
       <c r="M8" t="n">
-        <v>450.6129264831543</v>
+        <v>2277.501535415649</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>RL</t>
         </is>
       </c>
     </row>
@@ -841,31 +841,31 @@
         <v>3.0901</v>
       </c>
       <c r="E9" t="n">
-        <v>3.0901</v>
+        <v>4.17596</v>
       </c>
       <c r="F9" t="n">
-        <v>7</v>
+        <v>10.312</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9624</v>
+        <v>0.96035</v>
       </c>
       <c r="H9" t="n">
-        <v>84.82637405395508</v>
+        <v>567.2167778015137</v>
       </c>
       <c r="I9" t="n">
         <v>3.0901</v>
       </c>
       <c r="J9" t="n">
-        <v>7.361280000000001</v>
+        <v>5.649500000000001</v>
       </c>
       <c r="K9" t="n">
-        <v>16.7</v>
+        <v>12.632</v>
       </c>
       <c r="L9" t="n">
-        <v>0.9270860000000001</v>
+        <v>0.942738</v>
       </c>
       <c r="M9" t="n">
-        <v>375.5607128143311</v>
+        <v>1690.570449829102</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -896,7 +896,7 @@
         <v>0.9802999999999999</v>
       </c>
       <c r="H10" t="n">
-        <v>70.46298980712891</v>
+        <v>501.8974304199219</v>
       </c>
       <c r="I10" t="n">
         <v>2.4549</v>
@@ -911,7 +911,7 @@
         <v>0.9802999999999999</v>
       </c>
       <c r="M10" t="n">
-        <v>378.3904552459717</v>
+        <v>1342.992305755615</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -933,35 +933,35 @@
         <v>2.9062</v>
       </c>
       <c r="E11" t="n">
-        <v>3.96672</v>
+        <v>3.47</v>
       </c>
       <c r="F11" t="n">
-        <v>8.559999999999999</v>
+        <v>6.467999999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>0.95978</v>
+        <v>0.9574279999999999</v>
       </c>
       <c r="H11" t="n">
-        <v>75.21448135375977</v>
+        <v>604.2985916137695</v>
       </c>
       <c r="I11" t="n">
         <v>2.9062</v>
       </c>
       <c r="J11" t="n">
-        <v>6.230199999999999</v>
+        <v>2.9062</v>
       </c>
       <c r="K11" t="n">
-        <v>13.93</v>
+        <v>5</v>
       </c>
       <c r="L11" t="n">
-        <v>0.9515419999999999</v>
+        <v>0.9678000000000001</v>
       </c>
       <c r="M11" t="n">
-        <v>393.0646419525146</v>
+        <v>1521.068859100342</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>RL</t>
         </is>
       </c>
     </row>
@@ -976,34 +976,34 @@
         <v>60</v>
       </c>
       <c r="D12" t="n">
-        <v>5.8136</v>
+        <v>6.3444</v>
       </c>
       <c r="E12" t="n">
-        <v>9.305160000000001</v>
+        <v>7.831860000000001</v>
       </c>
       <c r="F12" t="n">
-        <v>23.704</v>
+        <v>20.544</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8736900000000001</v>
+        <v>0.9077019999999999</v>
       </c>
       <c r="H12" t="n">
-        <v>86.89494132995605</v>
+        <v>869.7157382965088</v>
       </c>
       <c r="I12" t="n">
-        <v>5.5247</v>
+        <v>8.6952</v>
       </c>
       <c r="J12" t="n">
-        <v>9.72444</v>
+        <v>11.06642</v>
       </c>
       <c r="K12" t="n">
-        <v>22.096</v>
+        <v>28.61</v>
       </c>
       <c r="L12" t="n">
-        <v>0.8808480000000001</v>
+        <v>0.8652979999999999</v>
       </c>
       <c r="M12" t="n">
-        <v>548.4851360321045</v>
+        <v>5391.840791702271</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1022,38 +1022,38 @@
         <v>181</v>
       </c>
       <c r="D13" t="n">
-        <v>7.5248</v>
+        <v>5.5382</v>
       </c>
       <c r="E13" t="n">
-        <v>10.13722</v>
+        <v>7.557220000000001</v>
       </c>
       <c r="F13" t="n">
-        <v>24.966</v>
+        <v>16.086</v>
       </c>
       <c r="G13" t="n">
-        <v>0.8896499999999999</v>
+        <v>0.9079360000000001</v>
       </c>
       <c r="H13" t="n">
-        <v>78.5029411315918</v>
+        <v>516.724157333374</v>
       </c>
       <c r="I13" t="n">
         <v>7.6853</v>
       </c>
       <c r="J13" t="n">
-        <v>9.726479999999999</v>
+        <v>12.50538</v>
       </c>
       <c r="K13" t="n">
-        <v>23.01</v>
+        <v>30.58</v>
       </c>
       <c r="L13" t="n">
-        <v>0.8846740000000001</v>
+        <v>0.8839980000000001</v>
       </c>
       <c r="M13" t="n">
-        <v>531.5917491912842</v>
+        <v>2419.676208496094</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>RL</t>
+          <t>GA</t>
         </is>
       </c>
     </row>
@@ -1068,34 +1068,34 @@
         <v>56</v>
       </c>
       <c r="D14" t="n">
-        <v>5.983</v>
+        <v>5.9011</v>
       </c>
       <c r="E14" t="n">
-        <v>8.016160000000001</v>
+        <v>8.22034</v>
       </c>
       <c r="F14" t="n">
-        <v>19.504</v>
+        <v>21.474</v>
       </c>
       <c r="G14" t="n">
-        <v>0.8965119999999999</v>
+        <v>0.8973479999999998</v>
       </c>
       <c r="H14" t="n">
-        <v>86.43126487731934</v>
+        <v>721.5856075286865</v>
       </c>
       <c r="I14" t="n">
-        <v>7.6566</v>
+        <v>3.8941</v>
       </c>
       <c r="J14" t="n">
-        <v>11.7565</v>
+        <v>10.95962</v>
       </c>
       <c r="K14" t="n">
-        <v>30.648</v>
+        <v>29.08</v>
       </c>
       <c r="L14" t="n">
-        <v>0.881578</v>
+        <v>0.900806</v>
       </c>
       <c r="M14" t="n">
-        <v>618.1217670440674</v>
+        <v>2429.720067977905</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1114,34 +1114,34 @@
         <v>148</v>
       </c>
       <c r="D15" t="n">
-        <v>6.057</v>
+        <v>5.727</v>
       </c>
       <c r="E15" t="n">
-        <v>8.203000000000001</v>
+        <v>6.432720000000001</v>
       </c>
       <c r="F15" t="n">
-        <v>19.306</v>
+        <v>14</v>
       </c>
       <c r="G15" t="n">
-        <v>0.920848</v>
+        <v>0.9330539999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>90.18635749816895</v>
+        <v>620.8535671234131</v>
       </c>
       <c r="I15" t="n">
-        <v>7.2426</v>
+        <v>6.4665</v>
       </c>
       <c r="J15" t="n">
-        <v>13.58596</v>
+        <v>11.42892</v>
       </c>
       <c r="K15" t="n">
-        <v>30.936</v>
+        <v>26.778</v>
       </c>
       <c r="L15" t="n">
-        <v>0.857198</v>
+        <v>0.887736</v>
       </c>
       <c r="M15" t="n">
-        <v>720.4530715942383</v>
+        <v>2527.234029769897</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
@@ -1163,35 +1163,35 @@
         <v>2.713</v>
       </c>
       <c r="E16" t="n">
-        <v>4.20676</v>
+        <v>2.713</v>
       </c>
       <c r="F16" t="n">
-        <v>8.407999999999999</v>
+        <v>4</v>
       </c>
       <c r="G16" t="n">
-        <v>0.938926</v>
+        <v>0.9513999999999999</v>
       </c>
       <c r="H16" t="n">
-        <v>79.85448837280273</v>
+        <v>693.2019233703613</v>
       </c>
       <c r="I16" t="n">
         <v>2.713</v>
       </c>
       <c r="J16" t="n">
-        <v>2.713</v>
+        <v>5.306420000000001</v>
       </c>
       <c r="K16" t="n">
-        <v>4</v>
+        <v>11.01</v>
       </c>
       <c r="L16" t="n">
-        <v>0.9513999999999999</v>
+        <v>0.9264720000000001</v>
       </c>
       <c r="M16" t="n">
-        <v>449.8175621032715</v>
+        <v>2056.155824661255</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>RL</t>
+          <t>GA</t>
         </is>
       </c>
     </row>
@@ -1206,34 +1206,34 @@
         <v>214</v>
       </c>
       <c r="D17" t="n">
-        <v>5.9406</v>
+        <v>6.4914</v>
       </c>
       <c r="E17" t="n">
-        <v>8.2628</v>
+        <v>8.06854</v>
       </c>
       <c r="F17" t="n">
-        <v>19.148</v>
+        <v>20.782</v>
       </c>
       <c r="G17" t="n">
-        <v>0.9157580000000001</v>
+        <v>0.8963000000000001</v>
       </c>
       <c r="H17" t="n">
-        <v>100.1801490783691</v>
+        <v>729.2549133300781</v>
       </c>
       <c r="I17" t="n">
-        <v>6.1951</v>
+        <v>8.081</v>
       </c>
       <c r="J17" t="n">
-        <v>10.29052</v>
+        <v>11.60004</v>
       </c>
       <c r="K17" t="n">
-        <v>22.75</v>
+        <v>30.836</v>
       </c>
       <c r="L17" t="n">
-        <v>0.88565</v>
+        <v>0.877322</v>
       </c>
       <c r="M17" t="n">
-        <v>527.2913932800293</v>
+        <v>2727.83031463623</v>
       </c>
       <c r="N17" t="inlineStr">
         <is>
@@ -1255,31 +1255,31 @@
         <v>3.4911</v>
       </c>
       <c r="E18" t="n">
-        <v>4.1409</v>
+        <v>5.208979999999999</v>
       </c>
       <c r="F18" t="n">
-        <v>9.42</v>
+        <v>12.486</v>
       </c>
       <c r="G18" t="n">
-        <v>0.961388</v>
+        <v>0.9550959999999999</v>
       </c>
       <c r="H18" t="n">
-        <v>77.73127555847168</v>
+        <v>492.8718090057373</v>
       </c>
       <c r="I18" t="n">
         <v>3.4911</v>
       </c>
       <c r="J18" t="n">
-        <v>8.030480000000001</v>
+        <v>9.447660000000001</v>
       </c>
       <c r="K18" t="n">
-        <v>20.414</v>
+        <v>21.622</v>
       </c>
       <c r="L18" t="n">
-        <v>0.9251280000000002</v>
+        <v>0.9321619999999999</v>
       </c>
       <c r="M18" t="n">
-        <v>445.9232330322266</v>
+        <v>1924.850225448608</v>
       </c>
       <c r="N18" t="inlineStr">
         <is>
@@ -1301,31 +1301,31 @@
         <v>2.0148</v>
       </c>
       <c r="E19" t="n">
-        <v>5.9382</v>
+        <v>2.71706</v>
       </c>
       <c r="F19" t="n">
-        <v>14.09</v>
+        <v>6.802</v>
       </c>
       <c r="G19" t="n">
-        <v>0.925084</v>
+        <v>0.948878</v>
       </c>
       <c r="H19" t="n">
-        <v>87.4455451965332</v>
+        <v>677.0806312561035</v>
       </c>
       <c r="I19" t="n">
         <v>2.0148</v>
       </c>
       <c r="J19" t="n">
-        <v>3.3364</v>
+        <v>2.0148</v>
       </c>
       <c r="K19" t="n">
-        <v>8.625999999999999</v>
+        <v>5</v>
       </c>
       <c r="L19" t="n">
-        <v>0.9479520000000001</v>
+        <v>0.9576</v>
       </c>
       <c r="M19" t="n">
-        <v>367.4840450286865</v>
+        <v>1139.173126220703</v>
       </c>
       <c r="N19" t="inlineStr">
         <is>
@@ -1344,34 +1344,34 @@
         <v>140</v>
       </c>
       <c r="D20" t="n">
-        <v>7.9084</v>
+        <v>4.8565</v>
       </c>
       <c r="E20" t="n">
-        <v>9.37036</v>
+        <v>6.650359999999999</v>
       </c>
       <c r="F20" t="n">
-        <v>19.964</v>
+        <v>17.21</v>
       </c>
       <c r="G20" t="n">
-        <v>0.883614</v>
+        <v>0.894814</v>
       </c>
       <c r="H20" t="n">
-        <v>85.2327823638916</v>
+        <v>699.1607189178467</v>
       </c>
       <c r="I20" t="n">
-        <v>13.8339</v>
+        <v>6.9128</v>
       </c>
       <c r="J20" t="n">
-        <v>16.406</v>
+        <v>9.043600000000001</v>
       </c>
       <c r="K20" t="n">
-        <v>39.592</v>
+        <v>22.816</v>
       </c>
       <c r="L20" t="n">
-        <v>0.836028</v>
+        <v>0.876622</v>
       </c>
       <c r="M20" t="n">
-        <v>755.3689956665039</v>
+        <v>2314.75396156311</v>
       </c>
       <c r="N20" t="inlineStr">
         <is>
@@ -1390,38 +1390,38 @@
         <v>70</v>
       </c>
       <c r="D21" t="n">
-        <v>4.2716</v>
+        <v>4.8496</v>
       </c>
       <c r="E21" t="n">
-        <v>6.388339999999999</v>
+        <v>9.13918</v>
       </c>
       <c r="F21" t="n">
-        <v>14.194</v>
+        <v>20.46</v>
       </c>
       <c r="G21" t="n">
-        <v>0.908224</v>
+        <v>0.89376</v>
       </c>
       <c r="H21" t="n">
-        <v>85.12754440307617</v>
+        <v>550.2259731292725</v>
       </c>
       <c r="I21" t="n">
-        <v>6.7217</v>
+        <v>4.9264</v>
       </c>
       <c r="J21" t="n">
-        <v>9.225599999999998</v>
+        <v>8.4598</v>
       </c>
       <c r="K21" t="n">
-        <v>21.26</v>
+        <v>18.528</v>
       </c>
       <c r="L21" t="n">
-        <v>0.896602</v>
+        <v>0.885426</v>
       </c>
       <c r="M21" t="n">
-        <v>563.0006790161133</v>
+        <v>2064.321327209473</v>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>RL</t>
         </is>
       </c>
     </row>

</xml_diff>